<commit_message>
Added Ship.java and a template Excel
</commit_message>
<xml_diff>
--- a/Ships.xlsx
+++ b/Ships.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Files\Documents\GitHub\Azur-Lane-Priority-Ship-Calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dai Nguyen\Documents\GitHub\Azur-Lane-Priority-Ship-Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2506E51-8B06-4666-8917-9F9F992A3973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CAC682-483C-4FCD-B914-90CBD872F57D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25EF0C69-8124-418B-83CF-5C04050B6A87}"/>
+    <workbookView xWindow="5760" yWindow="1368" windowWidth="17280" windowHeight="8964" xr2:uid="{25EF0C69-8124-418B-83CF-5C04050B6A87}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Iron Blood" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,12 +31,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Ship Type</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t>Z23</t>
+  </si>
+  <si>
+    <t>Z25</t>
+  </si>
+  <si>
+    <t>Konigsberg</t>
+  </si>
+  <si>
+    <t>Karlsruhe</t>
+  </si>
+  <si>
+    <t>Koln</t>
+  </si>
+  <si>
+    <t>Leipzig</t>
+  </si>
+  <si>
+    <t>Admiral Hipper</t>
+  </si>
+  <si>
+    <t>Prinz Eugen</t>
+  </si>
+  <si>
+    <t>Deutschland</t>
+  </si>
+  <si>
+    <t>Admiral Graf Spee</t>
+  </si>
+  <si>
+    <t>Scharnhorst</t>
+  </si>
+  <si>
+    <t>Gneisenau</t>
+  </si>
+  <si>
+    <t>Bismarck</t>
+  </si>
+  <si>
+    <t>Tirpiz</t>
+  </si>
+  <si>
+    <t>Graf Zeppelin</t>
+  </si>
+  <si>
+    <t>Z19</t>
+  </si>
+  <si>
+    <t>Z20</t>
+  </si>
+  <si>
+    <t>Z21</t>
+  </si>
+  <si>
+    <t>Z46</t>
+  </si>
+  <si>
+    <t>Z35</t>
+  </si>
+  <si>
+    <t>Z18</t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t>Zeppy</t>
+  </si>
+  <si>
+    <t>Z36</t>
+  </si>
+  <si>
+    <t>Roon</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Retrofit</t>
+  </si>
+  <si>
+    <t>Rarity</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Elite</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>SSR</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
   <si>
     <t>Modifier</t>
@@ -391,19 +514,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F3C672-B9A1-48D6-AE5E-F5FE826D0B82}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +535,455 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more classes Imported Apache POI 4.1.1
</commit_message>
<xml_diff>
--- a/Ships.xlsx
+++ b/Ships.xlsx
@@ -8,12 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dai Nguyen\Documents\GitHub\Azur-Lane-Priority-Ship-Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CAC682-483C-4FCD-B914-90CBD872F57D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D499ECFF-32D9-441B-909E-566E9F797857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1368" windowWidth="17280" windowHeight="8964" xr2:uid="{25EF0C69-8124-418B-83CF-5C04050B6A87}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{25EF0C69-8124-418B-83CF-5C04050B6A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Iron Blood" sheetId="1" r:id="rId1"/>
+    <sheet name="Sakura Empire" sheetId="2" r:id="rId2"/>
+    <sheet name="Eagle Union" sheetId="3" r:id="rId3"/>
+    <sheet name="Vichya Dominion" sheetId="7" r:id="rId4"/>
+    <sheet name="Royal Navy" sheetId="4" r:id="rId5"/>
+    <sheet name="Iris Libre" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -516,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F3C672-B9A1-48D6-AE5E-F5FE826D0B82}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -989,4 +994,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE41A06-0E2C-48EC-A746-F86D97E9C314}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BBB8AA-0172-42C3-A83C-02162B385706}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687616D3-B51E-400F-9E54-99AED3DC1912}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5776DAE-BA90-4DF2-BE61-C987D2B006BF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58DEF59-9199-4D14-BFF5-6AD296E6DDCA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Moving to other PC
</commit_message>
<xml_diff>
--- a/Ships.xlsx
+++ b/Ships.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dai Nguyen\Documents\GitHub\Azur-Lane-Priority-Ship-Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D499ECFF-32D9-441B-909E-566E9F797857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE68373-55C7-4BCF-8B9A-7840BCE4F8BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{25EF0C69-8124-418B-83CF-5C04050B6A87}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{25EF0C69-8124-418B-83CF-5C04050B6A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Iron Blood" sheetId="1" r:id="rId1"/>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F3C672-B9A1-48D6-AE5E-F5FE826D0B82}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,7 +580,7 @@
         <v>37</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1012,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BBB8AA-0172-42C3-A83C-02162B385706}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
Bugfix Limit Break Section
</commit_message>
<xml_diff>
--- a/Ships.xlsx
+++ b/Ships.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dai Nguyen\Documents\GitHub\Azur-Lane-Priority-Ship-Calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Files\Documents\GitHub\Azur_Lane_Priority_Ship_Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE68373-55C7-4BCF-8B9A-7840BCE4F8BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B51991-8752-42F9-8A13-D36B896E49C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{25EF0C69-8124-418B-83CF-5C04050B6A87}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{25EF0C69-8124-418B-83CF-5C04050B6A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Iron Blood" sheetId="1" r:id="rId1"/>
@@ -522,17 +522,17 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="J5" sqref="J5:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +549,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -566,7 +566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -580,10 +580,10 @@
         <v>37</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -600,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -617,7 +617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -634,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -651,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -702,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -719,7 +719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -736,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -855,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -889,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -923,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -940,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1002,7 +1002,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1014,7 +1014,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1026,7 +1026,7 @@
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1038,7 +1038,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1052,7 +1052,7 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>